<commit_message>
copy file to Shared directory-code update
</commit_message>
<xml_diff>
--- a/src/test/resources/TNData.xlsx
+++ b/src/test/resources/TNData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="107">
   <si>
     <t>TelephoneNumber</t>
   </si>
@@ -178,6 +178,174 @@
   </si>
   <si>
     <t>8039294009</t>
+  </si>
+  <si>
+    <t>4076840000</t>
+  </si>
+  <si>
+    <t>AIRESPRING, INC.</t>
+  </si>
+  <si>
+    <t>4076840001</t>
+  </si>
+  <si>
+    <t>4076840002</t>
+  </si>
+  <si>
+    <t>4076840003</t>
+  </si>
+  <si>
+    <t>4076840004</t>
+  </si>
+  <si>
+    <t>4076840005</t>
+  </si>
+  <si>
+    <t>4076840006</t>
+  </si>
+  <si>
+    <t>4076840007</t>
+  </si>
+  <si>
+    <t>4076840008</t>
+  </si>
+  <si>
+    <t>4076840009</t>
+  </si>
+  <si>
+    <t>9492093000</t>
+  </si>
+  <si>
+    <t>NEUTRAL TANDEM-CALIFORNIA, LLC - CA</t>
+  </si>
+  <si>
+    <t>9492093001</t>
+  </si>
+  <si>
+    <t>PAC - WEST TELECOMM, INC.</t>
+  </si>
+  <si>
+    <t>9492093002</t>
+  </si>
+  <si>
+    <t>9492093003</t>
+  </si>
+  <si>
+    <t>9492093004</t>
+  </si>
+  <si>
+    <t>9492093005</t>
+  </si>
+  <si>
+    <t>9492093006</t>
+  </si>
+  <si>
+    <t>9492093007</t>
+  </si>
+  <si>
+    <t>9492093008</t>
+  </si>
+  <si>
+    <t>9492093009</t>
+  </si>
+  <si>
+    <t>5044280000</t>
+  </si>
+  <si>
+    <t>BELLSOUTH TELECOMM INC DBA SOUTH CENTRAL BELL TEL</t>
+  </si>
+  <si>
+    <t>5044280001</t>
+  </si>
+  <si>
+    <t>5044280002</t>
+  </si>
+  <si>
+    <t>5044280003</t>
+  </si>
+  <si>
+    <t>5044280004</t>
+  </si>
+  <si>
+    <t>5044280005</t>
+  </si>
+  <si>
+    <t>5044280006</t>
+  </si>
+  <si>
+    <t>5044280007</t>
+  </si>
+  <si>
+    <t>5044280008</t>
+  </si>
+  <si>
+    <t>5044280009</t>
+  </si>
+  <si>
+    <t>2817540000</t>
+  </si>
+  <si>
+    <t>2817540001</t>
+  </si>
+  <si>
+    <t>2817540002</t>
+  </si>
+  <si>
+    <t>2817540003</t>
+  </si>
+  <si>
+    <t>2817540004</t>
+  </si>
+  <si>
+    <t>2817540005</t>
+  </si>
+  <si>
+    <t>2817540006</t>
+  </si>
+  <si>
+    <t>2817540007</t>
+  </si>
+  <si>
+    <t>2817540008</t>
+  </si>
+  <si>
+    <t>2817540009</t>
+  </si>
+  <si>
+    <t>2815044000</t>
+  </si>
+  <si>
+    <t>MCI WORLDCOM COMMUNICATIONS, INC. - TX</t>
+  </si>
+  <si>
+    <t>2815044001</t>
+  </si>
+  <si>
+    <t>LOGIX COMMUNICATIONS CORPORATION - TX</t>
+  </si>
+  <si>
+    <t>2815044002</t>
+  </si>
+  <si>
+    <t>2815044003</t>
+  </si>
+  <si>
+    <t>2815044004</t>
+  </si>
+  <si>
+    <t>2815044005</t>
+  </si>
+  <si>
+    <t>2815044006</t>
+  </si>
+  <si>
+    <t>2815044007</t>
+  </si>
+  <si>
+    <t>2815044008</t>
+  </si>
+  <si>
+    <t>2815044009</t>
   </si>
 </sst>
 </file>
@@ -194,7 +362,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="57">
+  <fills count="237">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,6 +386,906 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
         <fgColor indexed="55"/>
       </patternFill>
     </fill>
@@ -489,7 +1557,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="121">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
@@ -521,6 +1589,96 @@
     <xf applyFill="true" borderId="0" fillId="52" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="true" borderId="0" fillId="54" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="true" borderId="0" fillId="56" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="58" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="60" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="62" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="64" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="66" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="68" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="70" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="72" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="74" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="76" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="78" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="80" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="82" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="84" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="86" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="88" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="90" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="92" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="94" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="96" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="98" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="100" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="102" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="104" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="106" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="108" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="110" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="112" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="114" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="116" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="118" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="120" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="122" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="124" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="126" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="128" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="130" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="132" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="134" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="136" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="138" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="140" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="142" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="144" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="146" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="148" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="150" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="152" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="154" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="156" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="158" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="160" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="162" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="164" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="166" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="168" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="170" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="172" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="174" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="176" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="178" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="180" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="182" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="184" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="186" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="188" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="190" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="192" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="194" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="196" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="198" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="200" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="202" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="204" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="206" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="208" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="210" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="212" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="214" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="216" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="218" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="220" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="222" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="224" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="226" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="228" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="230" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="232" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="234" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="236" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -845,29 +2003,29 @@
     <col min="2" max="2" bestFit="true" customWidth="true" width="8.64453125" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="8.6796875" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="11.859375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="54.73828125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="43.40625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="116" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="117" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="120" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -879,12 +2037,12 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -896,12 +2054,12 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -913,12 +2071,12 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -930,12 +2088,12 @@
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>101</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -947,12 +2105,12 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>102</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -964,12 +2122,12 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>103</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -981,12 +2139,12 @@
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>104</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -998,12 +2156,12 @@
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>105</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -1015,12 +2173,12 @@
         <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>106</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -1032,7 +2190,7 @@
         <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>